<commit_message>
kezdetleges feltöltés és letöltés
</commit_message>
<xml_diff>
--- a/feladatok.xlsx
+++ b/feladatok.xlsx
@@ -470,7 +470,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -505,11 +505,17 @@
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
@@ -520,11 +526,17 @@
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
@@ -535,35 +547,56 @@
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>12</v>
       </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>13</v>
       </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>14</v>
+      </c>
+      <c r="B16">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feltöltés,letöltés bővítve; belépés, törlés, módosítás, keresés elkezdve;
</commit_message>
<xml_diff>
--- a/feladatok.xlsx
+++ b/feladatok.xlsx
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t>Rendszer</t>
   </si>
@@ -107,6 +107,12 @@
   </si>
   <si>
     <t>megjegyzés</t>
+  </si>
+  <si>
+    <t>Niki</t>
+  </si>
+  <si>
+    <t>esetleg online tárhellyel való megoldás keresése</t>
   </si>
 </sst>
 </file>
@@ -155,7 +161,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
@@ -165,6 +171,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -470,14 +479,14 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="D7" sqref="D7:D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -529,6 +538,12 @@
       <c r="B7">
         <v>1</v>
       </c>
+      <c r="C7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
@@ -537,6 +552,10 @@
       <c r="B8">
         <v>1</v>
       </c>
+      <c r="C8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="4"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
@@ -600,6 +619,9 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D7:D8"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
próbálkozom majd a módosítással.
</commit_message>
<xml_diff>
--- a/feladatok.xlsx
+++ b/feladatok.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -11,7 +11,7 @@
     <sheet name="Munka2" sheetId="2" r:id="rId2"/>
     <sheet name="Munka3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
   <si>
     <t>Rendszer</t>
   </si>
@@ -113,13 +113,16 @@
   </si>
   <si>
     <t>esetleg online tárhellyel való megoldás keresése</t>
+  </si>
+  <si>
+    <t>Tiha</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -264,7 +267,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -299,7 +301,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -475,21 +476,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" customWidth="1"/>
     <col min="4" max="4" width="25.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="B1" t="s">
         <v>15</v>
       </c>
@@ -500,17 +501,17 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -518,7 +519,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -529,12 +530,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
@@ -548,7 +549,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
@@ -560,12 +561,12 @@
       </c>
       <c r="D8" s="4"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
@@ -576,7 +577,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4">
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
@@ -587,15 +588,18 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B12">
         <v>2</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
       <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
@@ -606,7 +610,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="A14" s="3" t="s">
         <v>12</v>
       </c>
@@ -614,7 +618,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4">
       <c r="A15" s="3" t="s">
         <v>13</v>
       </c>
@@ -622,7 +626,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="A16" s="3" t="s">
         <v>14</v>
       </c>
@@ -640,24 +644,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>